<commit_message>
Cleaned up code for IC pw profiles and made plots more readable. Changed parameters to uM.
</commit_message>
<xml_diff>
--- a/index/data/incubationgraph.xlsx
+++ b/index/data/incubationgraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C4445B-B846-45BA-9E88-E83E1E5AD176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AD8FE3-C391-4D44-8D5C-1CEA2B6B11FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8251E3DC-A7BA-4CC3-B3AA-E4750F949FDE}"/>
   </bookViews>
@@ -1655,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3502AA23-6217-443D-8F96-C11B8D580A31}">
-  <dimension ref="A1:P353"/>
+  <dimension ref="A1:T353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="V328" sqref="V328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1672,7 @@
     <col min="15" max="15" width="9" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>144</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>661</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>23.186558525576821</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>662</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>34.978784165783381</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>663</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>39.906878463183126</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>664</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>69.827450983110197</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>665</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>75.811565487095606</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>666</v>
       </c>
@@ -2003,8 +2003,9 @@
       <c r="O7" s="7">
         <v>81.309720504525046</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>667</v>
       </c>
@@ -2050,8 +2051,9 @@
       <c r="O8" s="7">
         <v>89.154943822526235</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>668</v>
       </c>
@@ -2097,8 +2099,9 @@
       <c r="O9" s="7">
         <v>98.846102038880602</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>669</v>
       </c>
@@ -2144,8 +2147,9 @@
       <c r="O10" s="7">
         <v>96.53868341593909</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>670</v>
       </c>
@@ -2191,8 +2195,10 @@
       <c r="O11" s="7">
         <v>97.461650865115701</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R11" s="1"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>671</v>
       </c>
@@ -2238,8 +2244,10 @@
       <c r="O12" s="7">
         <v>90.645981153293278</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R12" s="1"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>672</v>
       </c>
@@ -2285,8 +2293,10 @@
       <c r="O13" s="7">
         <v>66.718995951859128</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13" s="1"/>
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>673</v>
       </c>
@@ -2332,8 +2342,10 @@
       <c r="O14" s="7">
         <v>40.680305294924722</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R14" s="1"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>674</v>
       </c>
@@ -2379,8 +2391,10 @@
       <c r="O15" s="7">
         <v>-0.94072803767676616</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R15" s="1"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>675</v>
       </c>
@@ -2426,8 +2440,10 @@
       <c r="O16" s="7">
         <v>-2.7799553698866522</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R16" s="1"/>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>676</v>
       </c>
@@ -2473,8 +2489,10 @@
       <c r="O17" s="7">
         <v>7.9450944136462004E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R17" s="1"/>
+      <c r="T17" s="7"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>677</v>
       </c>
@@ -2520,8 +2538,10 @@
       <c r="O18" s="7">
         <v>3.4077278395448975E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R18" s="1"/>
+      <c r="T18" s="7"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>678</v>
       </c>
@@ -2567,8 +2587,10 @@
       <c r="O19" s="7">
         <v>-5.6670053086573913E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R19" s="1"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>679</v>
       </c>
@@ -2614,8 +2636,10 @@
       <c r="O20" s="7">
         <v>-1.1296387345562469E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R20" s="1"/>
+      <c r="T20" s="7"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>680</v>
       </c>
@@ -2661,8 +2685,10 @@
       <c r="O21" s="7">
         <v>-0.10204371882758535</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R21" s="1"/>
+      <c r="T21" s="7"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>681</v>
       </c>
@@ -2681,11 +2707,16 @@
       <c r="F22" s="1">
         <v>54</v>
       </c>
+      <c r="G22" s="1">
+        <v>1.2</v>
+      </c>
       <c r="H22">
-        <v>17.8</v>
+        <f>19.6-1.8-G22</f>
+        <v>16.600000000000001</v>
       </c>
       <c r="I22" s="7">
-        <v>503.28314310508489</v>
+        <f>PI()*H22*9</f>
+        <v>469.3539424463151</v>
       </c>
       <c r="J22" s="7">
         <v>27.250446523960544</v>
@@ -2705,8 +2736,10 @@
       <c r="O22" s="7">
         <v>-3.7687035175311427</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R22" s="1"/>
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>682</v>
       </c>
@@ -2725,11 +2758,16 @@
       <c r="F23" s="1">
         <v>57</v>
       </c>
+      <c r="G23" s="1">
+        <v>0.9</v>
+      </c>
       <c r="H23">
-        <v>17.8</v>
+        <f>19.6-1.8-G23</f>
+        <v>16.900000000000002</v>
       </c>
       <c r="I23" s="7">
-        <v>503.28314310508489</v>
+        <f>PI()*H23*9</f>
+        <v>477.83624261100761</v>
       </c>
       <c r="J23" s="7">
         <v>24.613306537770864</v>
@@ -2749,8 +2787,10 @@
       <c r="O23" s="7">
         <v>-3.7687035175311427</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R23" s="1"/>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>687</v>
       </c>
@@ -2796,8 +2836,10 @@
       <c r="O24" s="7">
         <v>14.38639013736298</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R24" s="1"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>688</v>
       </c>
@@ -2843,8 +2885,10 @@
       <c r="O25" s="7">
         <v>24.770588835455317</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R25" s="1"/>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>689</v>
       </c>
@@ -2890,8 +2934,10 @@
       <c r="O26" s="7">
         <v>30.402696603912176</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R26" s="1"/>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>690</v>
       </c>
@@ -2937,8 +2983,10 @@
       <c r="O27" s="7">
         <v>61.379289330424911</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R27" s="1"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>691</v>
       </c>
@@ -2984,8 +3032,10 @@
       <c r="O28" s="7">
         <v>69.65144761534593</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R28" s="1"/>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>692</v>
       </c>
@@ -3031,8 +3081,10 @@
       <c r="O29" s="7">
         <v>72.080046012758984</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R29" s="1"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>693</v>
       </c>
@@ -3078,8 +3130,10 @@
       <c r="O30" s="7">
         <v>73.003013461935595</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R30" s="1"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>694</v>
       </c>
@@ -3126,7 +3180,7 @@
         <v>70.695594838994069</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>695</v>
       </c>
@@ -3173,7 +3227,7 @@
         <v>64.23482269475781</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>696</v>
       </c>
@@ -3219,8 +3273,9 @@
       <c r="O33" s="7">
         <v>62.850371520992887</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T33" s="7"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>697</v>
       </c>
@@ -3266,8 +3321,9 @@
       <c r="O34" s="7">
         <v>38.909197493537427</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T34" s="7"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>698</v>
       </c>
@@ -3313,8 +3369,9 @@
       <c r="O35" s="7">
         <v>5.0027010265940683</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T35" s="7"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>699</v>
       </c>
@@ -3360,8 +3417,9 @@
       <c r="O36" s="7">
         <v>-2.183909475189004</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T36" s="7"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>700</v>
       </c>
@@ -3407,8 +3465,10 @@
       <c r="O37" s="7">
         <v>-3.0183737277657112</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R37" s="1"/>
+      <c r="T37" s="7"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>701</v>
       </c>
@@ -3454,8 +3514,10 @@
       <c r="O38" s="7">
         <v>-2.3542083022454747</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R38" s="1"/>
+      <c r="T38" s="7"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>702</v>
       </c>
@@ -3501,8 +3563,10 @@
       <c r="O39" s="7">
         <v>1.1390445524944039E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R39" s="1"/>
+      <c r="T39" s="7"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>703</v>
       </c>
@@ -3548,8 +3612,10 @@
       <c r="O40" s="7">
         <v>0.60124810015809749</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R40" s="1"/>
+      <c r="T40" s="7"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>704</v>
       </c>
@@ -3595,8 +3661,10 @@
       <c r="O41" s="7">
         <v>-0.17010421743910331</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R41" s="1"/>
+      <c r="T41" s="7"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>705</v>
       </c>
@@ -3642,8 +3710,10 @@
       <c r="O42" s="7">
         <v>-3.3983220216067402E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R42" s="1"/>
+      <c r="T42" s="7"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>706</v>
       </c>
@@ -3689,8 +3759,10 @@
       <c r="O43" s="7">
         <v>1.0096110918272019</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R43" s="1"/>
+      <c r="T43" s="7"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>707</v>
       </c>
@@ -3709,11 +3781,16 @@
       <c r="F44" s="1">
         <v>54</v>
       </c>
+      <c r="G44" s="1">
+        <v>0.7</v>
+      </c>
       <c r="H44">
-        <v>13.2</v>
+        <f>18.2-5-G44</f>
+        <v>12.5</v>
       </c>
       <c r="I44" s="7">
-        <v>373.22120724646743</v>
+        <f>PI()*H44*9</f>
+        <v>353.42917352885172</v>
       </c>
       <c r="J44" s="7">
         <v>-29.887586510150225</v>
@@ -3733,8 +3810,10 @@
       <c r="O44" s="7">
         <v>-3.4360598147921673</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R44" s="1"/>
+      <c r="T44" s="7"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>708</v>
       </c>
@@ -3753,11 +3832,16 @@
       <c r="F45" s="1">
         <v>57</v>
       </c>
+      <c r="G45" s="1">
+        <v>0.8</v>
+      </c>
       <c r="H45">
-        <v>13.2</v>
+        <f>18.2-5-G45</f>
+        <v>12.399999999999999</v>
       </c>
       <c r="I45" s="7">
-        <v>373.22120724646743</v>
+        <f>PI()*H45*9</f>
+        <v>350.60174014062085</v>
       </c>
       <c r="J45" s="7">
         <v>1.758093324126534</v>
@@ -3777,8 +3861,10 @@
       <c r="O45" s="7">
         <v>-3.6855425918463971</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R45" s="1"/>
+      <c r="T45" s="7"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>713</v>
       </c>
@@ -3807,8 +3893,10 @@
         <v>681.4114465636261</v>
       </c>
       <c r="J46" s="10"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R46" s="1"/>
+      <c r="T46" s="7"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>714</v>
       </c>
@@ -3854,8 +3942,10 @@
       <c r="O47" s="7">
         <v>8.2262722656132876</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R47" s="1"/>
+      <c r="T47" s="7"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>715</v>
       </c>
@@ -3904,8 +3994,10 @@
       <c r="P48">
         <v>6.83</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R48" s="1"/>
+      <c r="T48" s="7"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>716</v>
       </c>
@@ -3954,8 +4046,10 @@
       <c r="P49">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R49" s="1"/>
+      <c r="T49" s="7"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>717</v>
       </c>
@@ -4004,8 +4098,10 @@
       <c r="P50">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R50" s="1"/>
+      <c r="T50" s="7"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>718</v>
       </c>
@@ -4054,8 +4150,10 @@
       <c r="P51">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R51" s="1"/>
+      <c r="T51" s="7"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>719</v>
       </c>
@@ -4104,8 +4202,10 @@
       <c r="P52">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R52" s="1"/>
+      <c r="T52" s="7"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>720</v>
       </c>
@@ -4154,8 +4254,10 @@
       <c r="P53">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R53" s="1"/>
+      <c r="T53" s="7"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>721</v>
       </c>
@@ -4204,8 +4306,10 @@
       <c r="P54">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R54" s="1"/>
+      <c r="T54" s="7"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>722</v>
       </c>
@@ -4254,8 +4358,10 @@
       <c r="P55">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R55" s="1"/>
+      <c r="T55" s="7"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>723</v>
       </c>
@@ -4304,8 +4410,10 @@
       <c r="P56">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R56" s="1"/>
+      <c r="T56" s="7"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>724</v>
       </c>
@@ -4354,8 +4462,10 @@
       <c r="P57">
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R57" s="1"/>
+      <c r="T57" s="7"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>725</v>
       </c>
@@ -4404,8 +4514,10 @@
       <c r="P58">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R58" s="1"/>
+      <c r="T58" s="7"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>726</v>
       </c>
@@ -4454,8 +4566,10 @@
       <c r="P59">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R59" s="1"/>
+      <c r="T59" s="7"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>727</v>
       </c>
@@ -4504,8 +4618,10 @@
       <c r="P60">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R60" s="1"/>
+      <c r="T60" s="7"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>728</v>
       </c>
@@ -4554,8 +4670,10 @@
       <c r="P61">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R61" s="1"/>
+      <c r="T61" s="7"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>729</v>
       </c>
@@ -4601,8 +4719,10 @@
       <c r="O62" s="7">
         <v>87.764059988641606</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R62" s="1"/>
+      <c r="T62" s="7"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>730</v>
       </c>
@@ -4648,8 +4768,10 @@
       <c r="O63" s="7">
         <v>92.687102721541393</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R63" s="1"/>
+      <c r="T63" s="7"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>731</v>
       </c>
@@ -4695,8 +4817,10 @@
       <c r="O64" s="7">
         <v>100.76361522344146</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R64" s="1"/>
+      <c r="T64" s="7"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>732</v>
       </c>
@@ -4742,8 +4866,10 @@
       <c r="O65" s="7">
         <v>100.37793906464286</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R65" s="1"/>
+      <c r="T65" s="7"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>733</v>
       </c>
@@ -4789,8 +4915,10 @@
       <c r="O66" s="7">
         <v>119.10156418167769</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R66" s="1"/>
+      <c r="T66" s="7"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>734</v>
       </c>
@@ -4836,8 +4964,10 @@
       <c r="O67" s="7">
         <v>120.22423667842172</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R67" s="1"/>
+      <c r="T67" s="7"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>739</v>
       </c>
@@ -4866,8 +4996,10 @@
         <v>783.19904853993535</v>
       </c>
       <c r="J68" s="10"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R68" s="1"/>
+      <c r="T68" s="7"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>740</v>
       </c>
@@ -4913,8 +5045,10 @@
       <c r="O69" s="7">
         <v>47.475023277047043</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R69" s="1"/>
+      <c r="T69" s="7"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>741</v>
       </c>
@@ -4960,8 +5094,10 @@
       <c r="O70" s="7">
         <v>39.730875095418853</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R70" s="1"/>
+      <c r="T70" s="7"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>742</v>
       </c>
@@ -5010,8 +5146,10 @@
       <c r="P71">
         <v>2.98</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R71" s="1"/>
+      <c r="T71" s="7"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>743</v>
       </c>
@@ -5060,8 +5198,10 @@
       <c r="P72">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R72" s="1"/>
+      <c r="T72" s="7"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>744</v>
       </c>
@@ -5110,8 +5250,10 @@
       <c r="P73">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R73" s="1"/>
+      <c r="T73" s="7"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>745</v>
       </c>
@@ -5160,8 +5302,10 @@
       <c r="P74">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R74" s="1"/>
+      <c r="T74" s="7"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>746</v>
       </c>
@@ -5210,8 +5354,10 @@
       <c r="P75">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R75" s="1"/>
+      <c r="T75" s="7"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>747</v>
       </c>
@@ -5260,8 +5406,10 @@
       <c r="P76">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R76" s="1"/>
+      <c r="T76" s="7"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>748</v>
       </c>
@@ -5310,8 +5458,10 @@
       <c r="P77">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R77" s="1"/>
+      <c r="T77" s="7"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>749</v>
       </c>
@@ -5360,8 +5510,10 @@
       <c r="P78">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R78" s="1"/>
+      <c r="T78" s="7"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>750</v>
       </c>
@@ -5410,8 +5562,10 @@
       <c r="P79">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R79" s="1"/>
+      <c r="T79" s="7"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>751</v>
       </c>
@@ -5460,8 +5614,10 @@
       <c r="P80">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R80" s="1"/>
+      <c r="T80" s="7"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>752</v>
       </c>
@@ -5510,8 +5666,10 @@
       <c r="P81">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R81" s="1"/>
+      <c r="T81" s="7"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>753</v>
       </c>
@@ -5560,8 +5718,10 @@
       <c r="P82">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R82" s="1"/>
+      <c r="T82" s="7"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>754</v>
       </c>
@@ -5610,8 +5770,10 @@
       <c r="P83">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R83" s="1"/>
+      <c r="T83" s="7"/>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>755</v>
       </c>
@@ -5657,8 +5819,10 @@
       <c r="O84" s="7">
         <v>85.971800191871637</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R84" s="1"/>
+      <c r="T84" s="7"/>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>756</v>
       </c>
@@ -5704,8 +5868,10 @@
       <c r="O85" s="7">
         <v>75.671978068661986</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R85" s="1"/>
+      <c r="T85" s="7"/>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>757</v>
       </c>
@@ -5751,8 +5917,10 @@
       <c r="O86" s="7">
         <v>87.355696996972483</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R86" s="1"/>
+      <c r="T86" s="7"/>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>758</v>
       </c>
@@ -5798,8 +5966,10 @@
       <c r="O87" s="7">
         <v>87.968241484476152</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R87" s="1"/>
+      <c r="T87" s="7"/>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>759</v>
       </c>
@@ -5845,8 +6015,10 @@
       <c r="O88" s="7">
         <v>94.236447401939316</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R88" s="1"/>
+      <c r="T88" s="7"/>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>760</v>
       </c>
@@ -5892,8 +6064,10 @@
       <c r="O89" s="7">
         <v>100.63983867966458</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R89" s="1"/>
+      <c r="T89" s="7"/>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>765</v>
       </c>
@@ -5939,8 +6113,10 @@
       <c r="O90" s="7">
         <v>6.6422419557347974</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R90" s="1"/>
+      <c r="T90" s="7"/>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>766</v>
       </c>
@@ -5986,8 +6162,10 @@
       <c r="O91" s="7">
         <v>7.1702520590276277</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R91" s="1"/>
+      <c r="T91" s="7"/>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>767</v>
       </c>
@@ -6033,8 +6211,10 @@
       <c r="O92" s="7">
         <v>9.4582958399632275</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R92" s="1"/>
+      <c r="T92" s="7"/>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>768</v>
       </c>
@@ -6080,8 +6260,10 @@
       <c r="O93" s="7">
         <v>17.378447389355689</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R93" s="1"/>
+      <c r="T93" s="7"/>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>769</v>
       </c>
@@ -6127,8 +6309,10 @@
       <c r="O94" s="7">
         <v>40.610891934240236</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R94" s="1"/>
+      <c r="T94" s="7"/>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>770</v>
       </c>
@@ -6174,8 +6358,10 @@
       <c r="O95" s="7">
         <v>19.009417685104026</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R95" s="1"/>
+      <c r="T95" s="7"/>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>771</v>
       </c>
@@ -6221,8 +6407,10 @@
       <c r="O96" s="7">
         <v>15.779031612985897</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R96" s="1"/>
+      <c r="T96" s="7"/>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>772</v>
       </c>
@@ -6268,8 +6456,10 @@
       <c r="O97" s="7">
         <v>9.3182594687496429</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R97" s="1"/>
+      <c r="T97" s="7"/>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>773</v>
       </c>
@@ -6315,8 +6505,10 @@
       <c r="O98" s="7">
         <v>8.3952920195730325</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R98" s="1"/>
+      <c r="T98" s="7"/>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>774</v>
       </c>
@@ -6362,8 +6554,10 @@
       <c r="O99" s="7">
         <v>6.5493571212198223</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R99" s="1"/>
+      <c r="T99" s="7"/>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>775</v>
       </c>
@@ -6409,8 +6603,10 @@
       <c r="O100" s="7">
         <v>5.1219102055335988</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R100" s="1"/>
+      <c r="T100" s="7"/>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>776</v>
       </c>
@@ -6456,8 +6652,10 @@
       <c r="O101" s="7">
         <v>0.31948328254111907</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R101" s="1"/>
+      <c r="T101" s="7"/>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>777</v>
       </c>
@@ -6503,8 +6701,10 @@
       <c r="O102" s="7">
         <v>0.86443952912182509</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R102" s="1"/>
+      <c r="T102" s="7"/>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>778</v>
       </c>
@@ -6550,8 +6750,10 @@
       <c r="O103" s="7">
         <v>0.40463269606935465</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R103" s="1"/>
+      <c r="T103" s="7"/>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>779</v>
       </c>
@@ -6597,8 +6799,10 @@
       <c r="O104" s="7">
         <v>-1.9284612346042973</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R104" s="1"/>
+      <c r="T104" s="7"/>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>780</v>
       </c>
@@ -6644,8 +6848,10 @@
       <c r="O105" s="7">
         <v>0.69199543164012034</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R105" s="1"/>
+      <c r="T105" s="7"/>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>781</v>
       </c>
@@ -6691,8 +6897,10 @@
       <c r="O106" s="7">
         <v>0.62393493302860092</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R106" s="1"/>
+      <c r="T106" s="7"/>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>782</v>
       </c>
@@ -6738,8 +6946,10 @@
       <c r="O107" s="7">
         <v>3.006052384431718</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R107" s="1"/>
+      <c r="T107" s="7"/>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>783</v>
       </c>
@@ -6785,8 +6995,10 @@
       <c r="O108" s="7">
         <v>1.4860345821078262</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R108" s="1"/>
+      <c r="T108" s="7"/>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>784</v>
       </c>
@@ -6833,7 +7045,7 @@
         <v>4.8209990140721857</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>785</v>
       </c>
@@ -6852,11 +7064,16 @@
       <c r="F110" s="1">
         <v>54</v>
       </c>
+      <c r="G110" s="1">
+        <v>0.9</v>
+      </c>
       <c r="H110">
-        <v>22.6</v>
+        <f>27.1-4.5-G110</f>
+        <v>21.700000000000003</v>
       </c>
       <c r="I110" s="7">
-        <v>638.99994574016398</v>
+        <f>PI()*H110*9</f>
+        <v>613.55304524608675</v>
       </c>
       <c r="J110" s="7">
         <v>108.1227394337788</v>
@@ -6877,7 +7094,7 @@
         <v>-1.6480999125701781</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>786</v>
       </c>
@@ -6896,11 +7113,16 @@
       <c r="F111" s="1">
         <v>57</v>
       </c>
+      <c r="G111" s="1">
+        <v>0.4</v>
+      </c>
       <c r="H111">
-        <v>22.6</v>
+        <f>27.1-4.5-G111</f>
+        <v>22.200000000000003</v>
       </c>
       <c r="I111" s="7">
-        <v>638.99994574016398</v>
+        <f>PI()*H111*9</f>
+        <v>627.69021218724072</v>
       </c>
       <c r="J111" s="7">
         <v>30.766633172213492</v>
@@ -6920,8 +7142,9 @@
       <c r="O111" s="7">
         <v>-3.2281575005803078</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T111" s="7"/>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>791</v>
       </c>
@@ -6967,8 +7190,9 @@
       <c r="O112" s="7">
         <v>8.9302857366703954</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T112" s="7"/>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>792</v>
       </c>
@@ -7014,8 +7238,9 @@
       <c r="O113" s="7">
         <v>17.906457492648517</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T113" s="7"/>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>793</v>
       </c>
@@ -7061,8 +7286,9 @@
       <c r="O114" s="7">
         <v>19.138481066998455</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T114" s="7"/>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>794</v>
       </c>
@@ -7108,8 +7334,10 @@
       <c r="O115" s="7">
         <v>42.722932347411557</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R115" s="1"/>
+      <c r="T115" s="7"/>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>795</v>
       </c>
@@ -7155,8 +7383,10 @@
       <c r="O116" s="7">
         <v>43.954955921761496</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R116" s="1"/>
+      <c r="T116" s="7"/>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>796</v>
       </c>
@@ -7202,8 +7432,10 @@
       <c r="O117" s="7">
         <v>45.775473711225658</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R117" s="1"/>
+      <c r="T117" s="7"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>797</v>
       </c>
@@ -7249,8 +7481,10 @@
       <c r="O118" s="7">
         <v>54.082180753815123</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R118" s="1"/>
+      <c r="T118" s="7"/>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>798</v>
       </c>
@@ -7296,8 +7530,10 @@
       <c r="O119" s="7">
         <v>57.774050550521558</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R119" s="1"/>
+      <c r="T119" s="7"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>799</v>
       </c>
@@ -7343,8 +7579,10 @@
       <c r="O120" s="7">
         <v>55.466631927580039</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R120" s="1"/>
+      <c r="T120" s="7"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>800</v>
       </c>
@@ -7390,8 +7628,10 @@
       <c r="O121" s="7">
         <v>56.389599376756642</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R121" s="1"/>
+      <c r="T121" s="7"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>801</v>
       </c>
@@ -7437,8 +7677,10 @@
       <c r="O122" s="7">
         <v>60.23061064100758</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R122" s="1"/>
+      <c r="T122" s="7"/>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>802</v>
       </c>
@@ -7484,8 +7726,10 @@
       <c r="O123" s="7">
         <v>38.040673475549426</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R123" s="1"/>
+      <c r="T123" s="7"/>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>803</v>
       </c>
@@ -7531,8 +7775,10 @@
       <c r="O124" s="7">
         <v>20.142266751914331</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R124" s="1"/>
+      <c r="T124" s="7"/>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>804</v>
       </c>
@@ -7578,8 +7824,10 @@
       <c r="O125" s="7">
         <v>-2.490447363890651</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R125" s="1"/>
+      <c r="T125" s="7"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>805</v>
       </c>
@@ -7625,8 +7873,10 @@
       <c r="O126" s="7">
         <v>-1.485684284257472</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R126" s="1"/>
+      <c r="T126" s="7"/>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>806</v>
       </c>
@@ -7672,8 +7922,10 @@
       <c r="O127" s="7">
         <v>-0.10204371882758535</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R127" s="1"/>
+      <c r="T127" s="7"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>807</v>
       </c>
@@ -7719,8 +7971,10 @@
       <c r="O128" s="7">
         <v>-0.10204371882758535</v>
       </c>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R128" s="1"/>
+      <c r="T128" s="7"/>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>808</v>
       </c>
@@ -7766,8 +8020,10 @@
       <c r="O129" s="7">
         <v>-1.1296387345562469E-2</v>
       </c>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R129" s="1"/>
+      <c r="T129" s="7"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>809</v>
       </c>
@@ -7813,8 +8069,10 @@
       <c r="O130" s="7">
         <v>-5.6670053086573913E-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R130" s="1"/>
+      <c r="T130" s="7"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>810</v>
       </c>
@@ -7860,8 +8118,10 @@
       <c r="O131" s="7">
         <v>0.21557194135949631</v>
       </c>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R131" s="1"/>
+      <c r="T131" s="7"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>811</v>
       </c>
@@ -7880,11 +8140,16 @@
       <c r="F132" s="1">
         <v>54</v>
       </c>
+      <c r="G132" s="1">
+        <v>1.6</v>
+      </c>
       <c r="H132">
-        <v>21.8</v>
+        <f>23-1.2-G132</f>
+        <v>20.2</v>
       </c>
       <c r="I132" s="7">
-        <v>616.38047863431746</v>
+        <f>PI()*H132*9</f>
+        <v>571.14154442262441</v>
       </c>
       <c r="J132" s="7">
         <v>75.598012937438895</v>
@@ -7904,8 +8169,10 @@
       <c r="O132" s="7">
         <v>-3.5608012033192833</v>
       </c>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R132" s="1"/>
+      <c r="T132" s="7"/>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>812</v>
       </c>
@@ -7924,11 +8191,16 @@
       <c r="F133" s="1">
         <v>57</v>
       </c>
+      <c r="G133" s="1">
+        <v>1.2</v>
+      </c>
       <c r="H133">
-        <v>21.8</v>
+        <f>23-1.2-G133</f>
+        <v>20.6</v>
       </c>
       <c r="I133" s="7">
-        <v>616.38047863431746</v>
+        <f>PI()*H133*9</f>
+        <v>582.45127797554778</v>
       </c>
       <c r="J133" s="7">
         <v>82.63038623394479</v>
@@ -7948,8 +8220,10 @@
       <c r="O133" s="7">
         <v>-3.5608012033192833</v>
       </c>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R133" s="1"/>
+      <c r="T133" s="7"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>817</v>
       </c>
@@ -7995,8 +8269,10 @@
       <c r="O134" s="7">
         <v>11.218329517605998</v>
       </c>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R134" s="1"/>
+      <c r="T134" s="7"/>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>818</v>
       </c>
@@ -8043,7 +8319,7 @@
         <v>16.498430550534305</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>819</v>
       </c>
@@ -8093,7 +8369,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>820</v>
       </c>
@@ -8142,8 +8418,9 @@
       <c r="P137">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T137" s="7"/>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>821</v>
       </c>
@@ -8192,8 +8469,9 @@
       <c r="P138">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T138" s="7"/>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>822</v>
       </c>
@@ -8242,8 +8520,9 @@
       <c r="P139">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T139" s="7"/>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>823</v>
       </c>
@@ -8292,8 +8571,9 @@
       <c r="P140">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T140" s="7"/>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>824</v>
       </c>
@@ -8342,8 +8622,10 @@
       <c r="P141">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R141" s="1"/>
+      <c r="T141" s="7"/>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>825</v>
       </c>
@@ -8392,8 +8674,10 @@
       <c r="P142">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R142" s="1"/>
+      <c r="T142" s="7"/>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>826</v>
       </c>
@@ -8442,8 +8726,10 @@
       <c r="P143">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R143" s="1"/>
+      <c r="T143" s="7"/>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>827</v>
       </c>
@@ -8492,8 +8778,10 @@
       <c r="P144">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R144" s="1"/>
+      <c r="T144" s="7"/>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>828</v>
       </c>
@@ -8542,8 +8830,10 @@
       <c r="P145">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R145" s="1"/>
+      <c r="T145" s="7"/>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>829</v>
       </c>
@@ -8592,8 +8882,10 @@
       <c r="P146">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R146" s="1"/>
+      <c r="T146" s="7"/>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>830</v>
       </c>
@@ -8642,8 +8934,10 @@
       <c r="P147">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R147" s="1"/>
+      <c r="T147" s="7"/>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>831</v>
       </c>
@@ -8692,8 +8986,10 @@
       <c r="P148">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R148" s="1"/>
+      <c r="T148" s="7"/>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>832</v>
       </c>
@@ -8742,8 +9038,10 @@
       <c r="P149">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R149" s="1"/>
+      <c r="T149" s="7"/>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>833</v>
       </c>
@@ -8789,8 +9087,10 @@
       <c r="O150" s="7">
         <v>84.678650718252811</v>
       </c>
-    </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R150" s="1"/>
+      <c r="T150" s="7"/>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>834</v>
       </c>
@@ -8836,8 +9136,10 @@
       <c r="O151" s="7">
         <v>88.081675648828664</v>
       </c>
-    </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R151" s="1"/>
+      <c r="T151" s="7"/>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>835</v>
       </c>
@@ -8883,8 +9185,10 @@
       <c r="O152" s="7">
         <v>86.652405177986807</v>
       </c>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R152" s="1"/>
+      <c r="T152" s="7"/>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>836</v>
       </c>
@@ -8930,8 +9234,10 @@
       <c r="O153" s="7">
         <v>88.626159637720832</v>
       </c>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R153" s="1"/>
+      <c r="T153" s="7"/>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>837</v>
       </c>
@@ -8977,8 +9283,10 @@
       <c r="O154" s="7">
         <v>133.90420895356209</v>
       </c>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R154" s="1"/>
+      <c r="T154" s="7"/>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>838</v>
       </c>
@@ -9024,8 +9332,10 @@
       <c r="O155" s="7">
         <v>99.683488034290036</v>
       </c>
-    </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R155" s="1"/>
+      <c r="T155" s="7"/>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>843</v>
       </c>
@@ -9054,8 +9364,10 @@
         <v>441.07960856400695</v>
       </c>
       <c r="J156" s="10"/>
-    </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R156" s="1"/>
+      <c r="T156" s="7"/>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>844</v>
       </c>
@@ -9101,8 +9413,10 @@
       <c r="O157" s="7">
         <v>27.410639351919471</v>
       </c>
-    </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R157" s="1"/>
+      <c r="T157" s="7"/>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>845</v>
       </c>
@@ -9148,8 +9462,10 @@
       <c r="O158" s="7">
         <v>32.16273028155495</v>
       </c>
-    </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R158" s="1"/>
+      <c r="T158" s="7"/>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>846</v>
       </c>
@@ -9198,8 +9514,10 @@
       <c r="P159">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R159" s="1"/>
+      <c r="T159" s="7"/>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>847</v>
       </c>
@@ -9248,8 +9566,10 @@
       <c r="P160">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R160" s="1"/>
+      <c r="T160" s="7"/>
+    </row>
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>848</v>
       </c>
@@ -9298,8 +9618,10 @@
       <c r="P161">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R161" s="1"/>
+      <c r="T161" s="7"/>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>849</v>
       </c>
@@ -9348,8 +9670,10 @@
       <c r="P162">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R162" s="1"/>
+      <c r="T162" s="7"/>
+    </row>
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>850</v>
       </c>
@@ -9398,8 +9722,10 @@
       <c r="P163">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R163" s="1"/>
+      <c r="T163" s="7"/>
+    </row>
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>851</v>
       </c>
@@ -9448,8 +9774,10 @@
       <c r="P164">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R164" s="1"/>
+      <c r="T164" s="7"/>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>852</v>
       </c>
@@ -9498,8 +9826,10 @@
       <c r="P165">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R165" s="1"/>
+      <c r="T165" s="7"/>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>853</v>
       </c>
@@ -9548,8 +9878,10 @@
       <c r="P166">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R166" s="1"/>
+      <c r="T166" s="7"/>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>854</v>
       </c>
@@ -9598,8 +9930,10 @@
       <c r="P167">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R167" s="1"/>
+      <c r="T167" s="7"/>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>855</v>
       </c>
@@ -9648,8 +9982,10 @@
       <c r="P168">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R168" s="1"/>
+      <c r="T168" s="7"/>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>856</v>
       </c>
@@ -9698,8 +10034,10 @@
       <c r="P169">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R169" s="1"/>
+      <c r="T169" s="7"/>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>857</v>
       </c>
@@ -9748,8 +10086,10 @@
       <c r="P170">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R170" s="1"/>
+      <c r="T170" s="7"/>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>858</v>
       </c>
@@ -9798,8 +10138,10 @@
       <c r="P171">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R171" s="1"/>
+      <c r="T171" s="7"/>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>859</v>
       </c>
@@ -9845,8 +10187,10 @@
       <c r="O172" s="7">
         <v>112.31121315452897</v>
       </c>
-    </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R172" s="1"/>
+      <c r="T172" s="7"/>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>860</v>
       </c>
@@ -9892,8 +10236,10 @@
       <c r="O173" s="7">
         <v>115.57811708788179</v>
       </c>
-    </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R173" s="1"/>
+      <c r="T173" s="7"/>
+    </row>
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>861</v>
       </c>
@@ -9939,8 +10285,10 @@
       <c r="O174" s="7">
         <v>113.40018113231322</v>
       </c>
-    </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R174" s="1"/>
+      <c r="T174" s="7"/>
+    </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>862</v>
       </c>
@@ -9986,8 +10334,10 @@
       <c r="O175" s="7">
         <v>115.2151277619537</v>
       </c>
-    </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R175" s="1"/>
+      <c r="T175" s="7"/>
+    </row>
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>863</v>
       </c>
@@ -10033,8 +10383,10 @@
       <c r="O176" s="7">
         <v>135.06846191314847</v>
       </c>
-    </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R176" s="1"/>
+      <c r="T176" s="7"/>
+    </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>864</v>
       </c>
@@ -10080,8 +10432,10 @@
       <c r="O177" s="7">
         <v>130.66093285185707</v>
       </c>
-    </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R177" s="1"/>
+      <c r="T177" s="7"/>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>869</v>
       </c>
@@ -10127,8 +10481,10 @@
       <c r="O178" s="7">
         <v>39.730875095418853</v>
       </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R178" s="1"/>
+      <c r="T178" s="7"/>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>870</v>
       </c>
@@ -10174,8 +10530,10 @@
       <c r="O179" s="7">
         <v>59.971262388310691</v>
       </c>
-    </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R179" s="1"/>
+      <c r="T179" s="7"/>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>871</v>
       </c>
@@ -10221,8 +10579,10 @@
       <c r="O180" s="7">
         <v>71.411481292988682</v>
       </c>
-    </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R180" s="1"/>
+      <c r="T180" s="7"/>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>872</v>
       </c>
@@ -10268,8 +10628,10 @@
       <c r="O181" s="7">
         <v>102.38807401950142</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R181" s="1"/>
+      <c r="T181" s="7"/>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>873</v>
       </c>
@@ -10315,8 +10677,10 @@
       <c r="O182" s="7">
         <v>100.62804034185865</v>
       </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R182" s="1"/>
+      <c r="T182" s="7"/>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>874</v>
       </c>
@@ -10362,8 +10726,10 @@
       <c r="O183" s="7">
         <v>115.45951612405955</v>
       </c>
-    </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R183" s="1"/>
+      <c r="T183" s="7"/>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>875</v>
       </c>
@@ -10409,8 +10775,10 @@
       <c r="O184" s="7">
         <v>95.615715966762494</v>
       </c>
-    </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R184" s="1"/>
+      <c r="T184" s="7"/>
+    </row>
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>876</v>
       </c>
@@ -10456,8 +10824,10 @@
       <c r="O185" s="7">
         <v>54.543664478403429</v>
       </c>
-    </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R185" s="1"/>
+      <c r="T185" s="7"/>
+    </row>
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>877</v>
       </c>
@@ -10503,8 +10873,10 @@
       <c r="O186" s="7">
         <v>35.622831770282964</v>
       </c>
-    </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R186" s="1"/>
+      <c r="T186" s="7"/>
+    </row>
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>878</v>
       </c>
@@ -10550,8 +10922,10 @@
       <c r="O187" s="7">
         <v>18.086450235927416</v>
       </c>
-    </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R187" s="1"/>
+      <c r="T187" s="7"/>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>879</v>
       </c>
@@ -10597,8 +10971,10 @@
       <c r="O188" s="7">
         <v>-1.9625210000155926</v>
       </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R188" s="1"/>
+      <c r="T188" s="7"/>
+    </row>
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>880</v>
       </c>
@@ -10644,8 +11020,10 @@
       <c r="O189" s="7">
         <v>-1.7581624075478262</v>
       </c>
-    </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R189" s="1"/>
+      <c r="T189" s="7"/>
+    </row>
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>881</v>
       </c>
@@ -10691,8 +11069,10 @@
       <c r="O190" s="7">
         <v>-1.7581624075478262</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R190" s="1"/>
+      <c r="T190" s="7"/>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>882</v>
       </c>
@@ -10738,8 +11118,10 @@
       <c r="O191" s="7">
         <v>1.4945451892307688</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R191" s="1"/>
+      <c r="T191" s="7"/>
+    </row>
+    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>883</v>
       </c>
@@ -10785,8 +11167,10 @@
       <c r="O192" s="7">
         <v>-0.77042921062029512</v>
       </c>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R192" s="1"/>
+      <c r="T192" s="7"/>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>884</v>
       </c>
@@ -10832,8 +11216,10 @@
       <c r="O193" s="7">
         <v>6.0687748219500088</v>
       </c>
-    </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R193" s="1"/>
+      <c r="T193" s="7"/>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>885</v>
       </c>
@@ -10879,8 +11265,10 @@
       <c r="O194" s="7">
         <v>2.2573868997050255</v>
       </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R194" s="1"/>
+      <c r="T194" s="7"/>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>886</v>
       </c>
@@ -10926,8 +11314,10 @@
       <c r="O195" s="7">
         <v>7.7476004543674435</v>
       </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R195" s="1"/>
+      <c r="T195" s="7"/>
+    </row>
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>887</v>
       </c>
@@ -10973,8 +11363,10 @@
       <c r="O196" s="7">
         <v>3.3236680446187998</v>
       </c>
-    </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R196" s="1"/>
+      <c r="T196" s="7"/>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>888</v>
       </c>
@@ -11020,8 +11412,10 @@
       <c r="O197" s="7">
         <v>4.2538281923095385</v>
       </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R197" s="1"/>
+      <c r="T197" s="7"/>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>889</v>
       </c>
@@ -11040,11 +11434,16 @@
       <c r="F198" s="1">
         <v>54</v>
       </c>
+      <c r="G198" s="1">
+        <v>1</v>
+      </c>
       <c r="H198">
-        <v>12.5</v>
+        <f>18-5.5-G198</f>
+        <v>11.5</v>
       </c>
       <c r="I198" s="7">
-        <v>353.42917352885172</v>
+        <f>PI()*H198*9</f>
+        <v>325.15483964654356</v>
       </c>
       <c r="J198" s="7">
         <v>201.30168561248243</v>
@@ -11064,8 +11463,10 @@
       <c r="O198" s="7">
         <v>3.5910384055686757</v>
       </c>
-    </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R198" s="1"/>
+      <c r="T198" s="7"/>
+    </row>
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>890</v>
       </c>
@@ -11084,11 +11485,16 @@
       <c r="F199" s="1">
         <v>57</v>
       </c>
+      <c r="G199" s="1">
+        <v>0.9</v>
+      </c>
       <c r="H199">
-        <v>12.5</v>
+        <f>18-5.5-G199</f>
+        <v>11.6</v>
       </c>
       <c r="I199" s="7">
-        <v>353.42917352885172</v>
+        <f>PI()*H199*9</f>
+        <v>327.98227303477438</v>
       </c>
       <c r="J199" s="7">
         <v>88.783712868387511</v>
@@ -11108,8 +11514,10 @@
       <c r="O199" s="7">
         <v>-1.7728413010972914</v>
       </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R199" s="1"/>
+      <c r="T199" s="7"/>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>895</v>
       </c>
@@ -11155,8 +11563,10 @@
       <c r="O200" s="7">
         <v>18.258464228177068</v>
       </c>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R200" s="1"/>
+      <c r="T200" s="7"/>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>896</v>
       </c>
@@ -11202,8 +11612,10 @@
       <c r="O201" s="7">
         <v>25.826609042040978</v>
       </c>
-    </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R201" s="1"/>
+      <c r="T201" s="7"/>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>897</v>
       </c>
@@ -11249,8 +11661,10 @@
       <c r="O202" s="7">
         <v>30.930706707205008</v>
       </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R202" s="1"/>
+      <c r="T202" s="7"/>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>898</v>
       </c>
@@ -11296,8 +11710,10 @@
       <c r="O203" s="7">
         <v>48.707046851396967</v>
       </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R203" s="1"/>
+      <c r="T203" s="7"/>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>899</v>
       </c>
@@ -11343,8 +11759,10 @@
       <c r="O204" s="7">
         <v>48.003033380339858</v>
       </c>
-    </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R204" s="1"/>
+      <c r="T204" s="7"/>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>900</v>
       </c>
@@ -11390,8 +11808,10 @@
       <c r="O205" s="7">
         <v>47.621408609578864</v>
       </c>
-    </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R205" s="1"/>
+      <c r="T205" s="7"/>
+    </row>
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>901</v>
       </c>
@@ -11437,8 +11857,10 @@
       <c r="O206" s="7">
         <v>39.776185291577704</v>
       </c>
-    </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R206" s="1"/>
+      <c r="T206" s="7"/>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>902</v>
       </c>
@@ -11484,8 +11906,10 @@
       <c r="O207" s="7">
         <v>23.624254930987064</v>
       </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R207" s="1"/>
+      <c r="T207" s="7"/>
+    </row>
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>903</v>
       </c>
@@ -11531,8 +11955,10 @@
       <c r="O208" s="7">
         <v>14.39458043922099</v>
       </c>
-    </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R208" s="1"/>
+      <c r="T208" s="7"/>
+    </row>
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>904</v>
       </c>
@@ -11578,8 +12004,10 @@
       <c r="O209" s="7">
         <v>10.24122691792625</v>
       </c>
-    </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R209" s="1"/>
+      <c r="T209" s="7"/>
+    </row>
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>905</v>
       </c>
@@ -11625,8 +12053,10 @@
       <c r="O210" s="7">
         <v>-1.877371586487357</v>
       </c>
-    </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R210" s="1"/>
+      <c r="T210" s="7"/>
+    </row>
+    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>906</v>
       </c>
@@ -11672,8 +12102,10 @@
       <c r="O211" s="7">
         <v>-2.8140151352979452</v>
       </c>
-    </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R211" s="1"/>
+      <c r="T211" s="7"/>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>907</v>
       </c>
@@ -11719,8 +12151,10 @@
       <c r="O212" s="7">
         <v>-2.183909475189004</v>
       </c>
-    </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R212" s="1"/>
+      <c r="T212" s="7"/>
+    </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>908</v>
       </c>
@@ -11767,7 +12201,7 @@
         <v>-0.53201085274123605</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>909</v>
       </c>
@@ -11814,7 +12248,7 @@
         <v>-3.0354036104713593</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>910</v>
       </c>
@@ -11860,8 +12294,9 @@
       <c r="O215" s="7">
         <v>-7.9356885957078849E-2</v>
       </c>
-    </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T215" s="7"/>
+    </row>
+    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>911</v>
       </c>
@@ -11907,8 +12342,9 @@
       <c r="O216" s="7">
         <v>0.10213777700696693</v>
       </c>
-    </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T216" s="7"/>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>912</v>
       </c>
@@ -11954,8 +12390,9 @@
       <c r="O217" s="7">
         <v>0.10213777700696693</v>
       </c>
-    </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T217" s="7"/>
+    </row>
+    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>913</v>
       </c>
@@ -12001,8 +12438,9 @@
       <c r="O218" s="7">
         <v>0.48781393580556653</v>
       </c>
-    </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T218" s="7"/>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>914</v>
       </c>
@@ -12048,8 +12486,10 @@
       <c r="O219" s="7">
         <v>0.64662176589910736</v>
       </c>
-    </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R219" s="1"/>
+      <c r="T219" s="7"/>
+    </row>
+    <row r="220" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>915</v>
       </c>
@@ -12068,11 +12508,16 @@
       <c r="F220" s="1">
         <v>54</v>
       </c>
+      <c r="G220" s="1">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H220">
-        <v>22.7</v>
+        <f>24.5-1.8-G220</f>
+        <v>20.5</v>
       </c>
       <c r="I220" s="7">
-        <v>641.82737912839468</v>
+        <f>PI()*H220*9</f>
+        <v>579.62384458731674</v>
       </c>
       <c r="J220" s="7">
         <v>75.598012937438895</v>
@@ -12092,8 +12537,10 @@
       <c r="O220" s="7">
         <v>-4.1845081459548616</v>
       </c>
-    </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R220" s="1"/>
+      <c r="T220" s="7"/>
+    </row>
+    <row r="221" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>916</v>
       </c>
@@ -12112,11 +12559,16 @@
       <c r="F221" s="1">
         <v>57</v>
       </c>
+      <c r="G221" s="1">
+        <v>1.4</v>
+      </c>
       <c r="H221">
-        <v>22.7</v>
+        <f>24.5-1.8-G221</f>
+        <v>21.3</v>
       </c>
       <c r="I221" s="7">
-        <v>641.82737912839468</v>
+        <f>PI()*H221*9</f>
+        <v>602.24331169316338</v>
       </c>
       <c r="J221" s="7">
         <v>74.718966275375621</v>
@@ -12136,8 +12588,10 @@
       <c r="O221" s="7">
         <v>-3.1865770377379348</v>
       </c>
-    </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R221" s="1"/>
+      <c r="T221" s="7"/>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>921</v>
       </c>
@@ -12183,8 +12637,10 @@
       <c r="O222" s="7">
         <v>63.491329743596239</v>
       </c>
-    </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R222" s="1"/>
+      <c r="T222" s="7"/>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>922</v>
       </c>
@@ -12230,8 +12686,10 @@
       <c r="O223" s="7">
         <v>66.307383627824663</v>
       </c>
-    </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R223" s="1"/>
+      <c r="T223" s="7"/>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>923</v>
       </c>
@@ -12280,8 +12738,10 @@
       <c r="P224">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R224" s="1"/>
+      <c r="T224" s="7"/>
+    </row>
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>924</v>
       </c>
@@ -12330,8 +12790,10 @@
       <c r="P225">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R225" s="1"/>
+      <c r="T225" s="7"/>
+    </row>
+    <row r="226" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>925</v>
       </c>
@@ -12380,8 +12842,10 @@
       <c r="P226">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R226" s="1"/>
+      <c r="T226" s="7"/>
+    </row>
+    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>926</v>
       </c>
@@ -12430,8 +12894,10 @@
       <c r="P227">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R227" s="1"/>
+      <c r="T227" s="7"/>
+    </row>
+    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>927</v>
       </c>
@@ -12480,8 +12946,10 @@
       <c r="P228">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R228" s="1"/>
+      <c r="T228" s="7"/>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>928</v>
       </c>
@@ -12530,8 +12998,10 @@
       <c r="P229">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R229" s="1"/>
+      <c r="T229" s="7"/>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>929</v>
       </c>
@@ -12580,8 +13050,10 @@
       <c r="P230">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R230" s="1"/>
+      <c r="T230" s="7"/>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>930</v>
       </c>
@@ -12630,8 +13102,10 @@
       <c r="P231">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R231" s="1"/>
+      <c r="T231" s="7"/>
+    </row>
+    <row r="232" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>931</v>
       </c>
@@ -12680,8 +13154,10 @@
       <c r="P232">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R232" s="1"/>
+      <c r="T232" s="7"/>
+    </row>
+    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>932</v>
       </c>
@@ -12730,8 +13206,10 @@
       <c r="P233">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R233" s="1"/>
+      <c r="T233" s="7"/>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>933</v>
       </c>
@@ -12780,8 +13258,10 @@
       <c r="P234">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R234" s="1"/>
+      <c r="T234" s="7"/>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>934</v>
       </c>
@@ -12830,8 +13310,10 @@
       <c r="P235">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R235" s="1"/>
+      <c r="T235" s="7"/>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>935</v>
       </c>
@@ -12880,8 +13362,10 @@
       <c r="P236">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R236" s="1"/>
+      <c r="T236" s="7"/>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>936</v>
       </c>
@@ -12930,8 +13414,10 @@
       <c r="P237">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R237" s="1"/>
+      <c r="T237" s="7"/>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>937</v>
       </c>
@@ -12977,8 +13463,10 @@
       <c r="O238" s="7">
         <v>117.61993204622732</v>
       </c>
-    </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R238" s="1"/>
+      <c r="T238" s="7"/>
+    </row>
+    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>938</v>
       </c>
@@ -13025,7 +13513,7 @@
         <v>128.26005666249458</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>939</v>
       </c>
@@ -13072,7 +13560,7 @@
         <v>129.39439830601984</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>940</v>
       </c>
@@ -13118,8 +13606,9 @@
       <c r="O241" s="7">
         <v>130.2791847879696</v>
       </c>
-    </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T241" s="7"/>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>941</v>
       </c>
@@ -13165,8 +13654,9 @@
       <c r="O242" s="7">
         <v>158.93564758466994</v>
       </c>
-    </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T242" s="7"/>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>942</v>
       </c>
@@ -13212,8 +13702,9 @@
       <c r="O243" s="7">
         <v>150.16216992492946</v>
       </c>
-    </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T243" s="7"/>
+    </row>
+    <row r="244" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>947</v>
       </c>
@@ -13242,8 +13733,9 @@
         <v>712.51321383416507</v>
       </c>
       <c r="J244" s="10"/>
-    </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T244" s="7"/>
+    </row>
+    <row r="245" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>948</v>
       </c>
@@ -13289,8 +13781,10 @@
       <c r="O245" s="7">
         <v>36.210807740133319</v>
       </c>
-    </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R245" s="1"/>
+      <c r="T245" s="7"/>
+    </row>
+    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>949</v>
       </c>
@@ -13339,8 +13833,10 @@
       <c r="P246">
         <v>5.32</v>
       </c>
-    </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R246" s="1"/>
+      <c r="T246" s="7"/>
+    </row>
+    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>950</v>
       </c>
@@ -13389,8 +13885,10 @@
       <c r="P247">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R247" s="1"/>
+      <c r="T247" s="7"/>
+    </row>
+    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>951</v>
       </c>
@@ -13439,8 +13937,10 @@
       <c r="P248">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R248" s="1"/>
+      <c r="T248" s="7"/>
+    </row>
+    <row r="249" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>952</v>
       </c>
@@ -13489,8 +13989,10 @@
       <c r="P249">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R249" s="1"/>
+      <c r="T249" s="7"/>
+    </row>
+    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>953</v>
       </c>
@@ -13539,8 +14041,10 @@
       <c r="P250">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R250" s="1"/>
+      <c r="T250" s="7"/>
+    </row>
+    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>954</v>
       </c>
@@ -13589,8 +14093,10 @@
       <c r="P251">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R251" s="1"/>
+      <c r="T251" s="7"/>
+    </row>
+    <row r="252" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>955</v>
       </c>
@@ -13639,8 +14145,10 @@
       <c r="P252">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R252" s="1"/>
+      <c r="T252" s="7"/>
+    </row>
+    <row r="253" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>956</v>
       </c>
@@ -13689,8 +14197,10 @@
       <c r="P253">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R253" s="1"/>
+      <c r="T253" s="7"/>
+    </row>
+    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>957</v>
       </c>
@@ -13739,8 +14249,10 @@
       <c r="P254">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R254" s="1"/>
+      <c r="T254" s="7"/>
+    </row>
+    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>958</v>
       </c>
@@ -13789,8 +14301,10 @@
       <c r="P255">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R255" s="1"/>
+      <c r="T255" s="7"/>
+    </row>
+    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>959</v>
       </c>
@@ -13839,8 +14353,10 @@
       <c r="P256">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R256" s="1"/>
+      <c r="T256" s="7"/>
+    </row>
+    <row r="257" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>960</v>
       </c>
@@ -13889,8 +14405,10 @@
       <c r="P257">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R257" s="1"/>
+      <c r="T257" s="7"/>
+    </row>
+    <row r="258" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>961</v>
       </c>
@@ -13939,8 +14457,10 @@
       <c r="P258">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R258" s="1"/>
+      <c r="T258" s="7"/>
+    </row>
+    <row r="259" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>962</v>
       </c>
@@ -13989,8 +14509,10 @@
       <c r="P259">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R259" s="1"/>
+      <c r="T259" s="7"/>
+    </row>
+    <row r="260" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>963</v>
       </c>
@@ -14036,8 +14558,10 @@
       <c r="O260" s="7">
         <v>110.42820602627695</v>
       </c>
-    </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R260" s="1"/>
+      <c r="T260" s="7"/>
+    </row>
+    <row r="261" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>964</v>
       </c>
@@ -14083,8 +14607,10 @@
       <c r="O261" s="7">
         <v>124.06299258145098</v>
       </c>
-    </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R261" s="1"/>
+      <c r="T261" s="7"/>
+    </row>
+    <row r="262" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>965</v>
       </c>
@@ -14130,8 +14656,10 @@
       <c r="O262" s="7">
         <v>130.80098194399122</v>
       </c>
-    </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R262" s="1"/>
+      <c r="T262" s="7"/>
+    </row>
+    <row r="263" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>966</v>
       </c>
@@ -14177,8 +14705,10 @@
       <c r="O263" s="7">
         <v>134.09057271021456</v>
       </c>
-    </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R263" s="1"/>
+      <c r="T263" s="7"/>
+    </row>
+    <row r="264" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>967</v>
       </c>
@@ -14224,8 +14754,10 @@
       <c r="O264" s="7">
         <v>152.61541723262943</v>
       </c>
-    </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R264" s="1"/>
+      <c r="T264" s="7"/>
+    </row>
+    <row r="265" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>968</v>
       </c>
@@ -14271,8 +14803,10 @@
       <c r="O265" s="7">
         <v>153.0728023238955</v>
       </c>
-    </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R265" s="1"/>
+      <c r="T265" s="7"/>
+    </row>
+    <row r="266" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>973</v>
       </c>
@@ -14318,8 +14852,10 @@
       <c r="O266" s="7">
         <v>31.282713442733563</v>
       </c>
-    </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R266" s="1"/>
+      <c r="T266" s="7"/>
+    </row>
+    <row r="267" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>974</v>
       </c>
@@ -14365,8 +14901,10 @@
       <c r="O267" s="7">
         <v>42.37092561188301</v>
       </c>
-    </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R267" s="1"/>
+      <c r="T267" s="7"/>
+    </row>
+    <row r="268" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>975</v>
       </c>
@@ -14412,8 +14950,10 @@
       <c r="O268" s="7">
         <v>54.51515798761811</v>
       </c>
-    </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R268" s="1"/>
+      <c r="T268" s="7"/>
+    </row>
+    <row r="269" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>976</v>
       </c>
@@ -14459,8 +14999,10 @@
       <c r="O269" s="7">
         <v>142.16483513422801</v>
       </c>
-    </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R269" s="1"/>
+      <c r="T269" s="7"/>
+    </row>
+    <row r="270" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>977</v>
       </c>
@@ -14506,8 +15048,10 @@
       <c r="O270" s="7">
         <v>79.859642945673983</v>
       </c>
-    </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R270" s="1"/>
+      <c r="T270" s="7"/>
+    </row>
+    <row r="271" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>978</v>
       </c>
@@ -14553,8 +15097,10 @@
       <c r="O271" s="7">
         <v>88.69346009793793</v>
       </c>
-    </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R271" s="1"/>
+      <c r="T271" s="7"/>
+    </row>
+    <row r="272" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>979</v>
       </c>
@@ -14600,8 +15146,10 @@
       <c r="O272" s="7">
         <v>92.385329894644357</v>
       </c>
-    </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R272" s="1"/>
+      <c r="T272" s="7"/>
+    </row>
+    <row r="273" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>980</v>
       </c>
@@ -14647,8 +15195,10 @@
       <c r="O273" s="7">
         <v>93.769781068409273</v>
       </c>
-    </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R273" s="1"/>
+      <c r="T273" s="7"/>
+    </row>
+    <row r="274" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>981</v>
       </c>
@@ -14694,8 +15244,10 @@
       <c r="O274" s="7">
         <v>85.463074025819793</v>
       </c>
-    </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R274" s="1"/>
+      <c r="T274" s="7"/>
+    </row>
+    <row r="275" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>982</v>
       </c>
@@ -14741,8 +15293,10 @@
       <c r="O275" s="7">
         <v>81.771204229113351</v>
       </c>
-    </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R275" s="1"/>
+      <c r="T275" s="7"/>
+    </row>
+    <row r="276" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>983</v>
       </c>
@@ -14788,8 +15342,10 @@
       <c r="O276" s="7">
         <v>67.417221142790652</v>
       </c>
-    </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R276" s="1"/>
+      <c r="T276" s="7"/>
+    </row>
+    <row r="277" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>984</v>
       </c>
@@ -14835,8 +15391,10 @@
       <c r="O277" s="7">
         <v>32.301603003746358</v>
       </c>
-    </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R277" s="1"/>
+      <c r="T277" s="7"/>
+    </row>
+    <row r="278" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>985</v>
       </c>
@@ -14882,8 +15440,10 @@
       <c r="O278" s="7">
         <v>3.1975334597954772</v>
       </c>
-    </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R278" s="1"/>
+      <c r="T278" s="7"/>
+    </row>
+    <row r="279" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>986</v>
       </c>
@@ -14929,8 +15489,10 @@
       <c r="O279" s="7">
         <v>-0.24250284674523442</v>
       </c>
-    </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R279" s="1"/>
+      <c r="T279" s="7"/>
+    </row>
+    <row r="280" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>987</v>
       </c>
@@ -14976,8 +15538,10 @@
       <c r="O280" s="7">
         <v>-1.2472659263784129</v>
       </c>
-    </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R280" s="1"/>
+      <c r="T280" s="7"/>
+    </row>
+    <row r="281" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>988</v>
       </c>
@@ -15023,8 +15587,10 @@
       <c r="O281" s="7">
         <v>2.8245577214676691</v>
       </c>
-    </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R281" s="1"/>
+      <c r="T281" s="7"/>
+    </row>
+    <row r="282" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>989</v>
       </c>
@@ -15070,8 +15636,10 @@
       <c r="O282" s="7">
         <v>3.0741128830432345</v>
       </c>
-    </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R282" s="1"/>
+      <c r="T282" s="7"/>
+    </row>
+    <row r="283" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>990</v>
       </c>
@@ -15117,8 +15685,10 @@
       <c r="O283" s="7">
         <v>2.6884367242446361</v>
       </c>
-    </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R283" s="1"/>
+      <c r="T283" s="7"/>
+    </row>
+    <row r="284" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>991</v>
       </c>
@@ -15164,8 +15734,10 @@
       <c r="O284" s="7">
         <v>3.4371022089713295</v>
       </c>
-    </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R284" s="1"/>
+      <c r="T284" s="7"/>
+    </row>
+    <row r="285" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>992</v>
       </c>
@@ -15211,8 +15783,10 @@
       <c r="O285" s="7">
         <v>2.5976893927626103</v>
       </c>
-    </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R285" s="1"/>
+      <c r="T285" s="7"/>
+    </row>
+    <row r="286" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>993</v>
       </c>
@@ -15231,11 +15805,16 @@
       <c r="F286" s="1">
         <v>54</v>
       </c>
+      <c r="G286" s="1">
+        <v>2</v>
+      </c>
       <c r="H286">
-        <v>24.5</v>
+        <f>26.5-2-G286</f>
+        <v>22.5</v>
       </c>
       <c r="I286" s="7">
-        <v>692.72118011654936</v>
+        <f>PI()*H286*9</f>
+        <v>636.17251235193316</v>
       </c>
       <c r="J286" s="7">
         <v>245.25401871564455</v>
@@ -15255,8 +15834,10 @@
       <c r="O286" s="7">
         <v>1.7199175776619404</v>
       </c>
-    </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R286" s="1"/>
+      <c r="T286" s="7"/>
+    </row>
+    <row r="287" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>994</v>
       </c>
@@ -15275,11 +15856,16 @@
       <c r="F287" s="1">
         <v>57</v>
       </c>
+      <c r="G287" s="1">
+        <v>0.4</v>
+      </c>
       <c r="H287">
-        <v>24.5</v>
+        <f>26.5-2-G287</f>
+        <v>24.1</v>
       </c>
       <c r="I287" s="7">
-        <v>692.72118011654936</v>
+        <f>PI()*H287*9</f>
+        <v>681.4114465636261</v>
       </c>
       <c r="J287" s="7">
         <v>46.589473089351934</v>
@@ -15299,8 +15885,10 @@
       <c r="O287" s="7">
         <v>-3.1865770377379348</v>
       </c>
-    </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R287" s="1"/>
+      <c r="T287" s="7"/>
+    </row>
+    <row r="288" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>999</v>
       </c>
@@ -15346,8 +15934,10 @@
       <c r="O288" s="7">
         <v>33.922763959197717</v>
       </c>
-    </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R288" s="1"/>
+      <c r="T288" s="7"/>
+    </row>
+    <row r="289" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>1000</v>
       </c>
@@ -15393,8 +15983,10 @@
       <c r="O289" s="7">
         <v>53.987147884325282</v>
       </c>
-    </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R289" s="1"/>
+      <c r="T289" s="7"/>
+    </row>
+    <row r="290" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>1001</v>
       </c>
@@ -15440,8 +16032,10 @@
       <c r="O290" s="7">
         <v>61.203285962660637</v>
       </c>
-    </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R290" s="1"/>
+      <c r="T290" s="7"/>
+    </row>
+    <row r="291" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>1002</v>
       </c>
@@ -15487,8 +16081,10 @@
       <c r="O291" s="7">
         <v>91.475865218116255</v>
       </c>
-    </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R291" s="1"/>
+      <c r="T291" s="7"/>
+    </row>
+    <row r="292" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>1003</v>
       </c>
@@ -15534,8 +16130,10 @@
       <c r="O292" s="7">
         <v>100.62804034185865</v>
       </c>
-    </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R292" s="1"/>
+      <c r="T292" s="7"/>
+    </row>
+    <row r="293" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>1004</v>
       </c>
@@ -15581,8 +16179,10 @@
       <c r="O293" s="7">
         <v>104.38390673394024</v>
       </c>
-    </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R293" s="1"/>
+      <c r="T293" s="7"/>
+    </row>
+    <row r="294" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>1005</v>
       </c>
@@ -15628,8 +16228,10 @@
       <c r="O294" s="7">
         <v>112.22913005194142</v>
       </c>
-    </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R294" s="1"/>
+      <c r="T294" s="7"/>
+    </row>
+    <row r="295" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>1006</v>
       </c>
@@ -15675,8 +16277,10 @@
       <c r="O295" s="7">
         <v>122.84325571747242</v>
       </c>
-    </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R295" s="1"/>
+      <c r="T295" s="7"/>
+    </row>
+    <row r="296" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>1007</v>
       </c>
@@ -15722,8 +16326,10 @@
       <c r="O296" s="7">
         <v>108.07577653064668</v>
       </c>
-    </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R296" s="1"/>
+      <c r="T296" s="7"/>
+    </row>
+    <row r="297" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>1008</v>
       </c>
@@ -15769,8 +16375,10 @@
       <c r="O297" s="7">
         <v>102.53797183558702</v>
       </c>
-    </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R297" s="1"/>
+      <c r="T297" s="7"/>
+    </row>
+    <row r="298" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>1009</v>
       </c>
@@ -15816,8 +16424,10 @@
       <c r="O298" s="7">
         <v>85.792464582183868</v>
       </c>
-    </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R298" s="1"/>
+      <c r="T298" s="7"/>
+    </row>
+    <row r="299" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>1010</v>
       </c>
@@ -15863,8 +16473,10 @@
       <c r="O299" s="7">
         <v>53.435687441454384</v>
       </c>
-    </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R299" s="1"/>
+      <c r="T299" s="7"/>
+    </row>
+    <row r="300" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>1011</v>
       </c>
@@ -15910,8 +16522,10 @@
       <c r="O300" s="7">
         <v>-1.877371586487357</v>
       </c>
-    </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R300" s="1"/>
+      <c r="T300" s="7"/>
+    </row>
+    <row r="301" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>1012</v>
       </c>
@@ -15957,8 +16571,10 @@
       <c r="O301" s="7">
         <v>-2.0136106481325329</v>
       </c>
-    </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R301" s="1"/>
+      <c r="T301" s="7"/>
+    </row>
+    <row r="302" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>1013</v>
       </c>
@@ -16004,8 +16620,10 @@
       <c r="O302" s="7">
         <v>-3.2057024375278278</v>
       </c>
-    </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R302" s="1"/>
+      <c r="T302" s="7"/>
+    </row>
+    <row r="303" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>1014</v>
       </c>
@@ -16051,8 +16669,10 @@
       <c r="O303" s="7">
         <v>1.1390445524944039E-2</v>
       </c>
-    </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R303" s="1"/>
+      <c r="T303" s="7"/>
+    </row>
+    <row r="304" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>1015</v>
       </c>
@@ -16098,8 +16718,10 @@
       <c r="O304" s="7">
         <v>-0.10204371882758535</v>
       </c>
-    </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R304" s="1"/>
+      <c r="T304" s="7"/>
+    </row>
+    <row r="305" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>1016</v>
       </c>
@@ -16145,8 +16767,10 @@
       <c r="O305" s="7">
         <v>0.32900610571202571</v>
       </c>
-    </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R305" s="1"/>
+      <c r="T305" s="7"/>
+    </row>
+    <row r="306" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>1017</v>
       </c>
@@ -16192,8 +16816,10 @@
       <c r="O306" s="7">
         <v>1.100358423309225</v>
       </c>
-    </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R306" s="1"/>
+      <c r="T306" s="7"/>
+    </row>
+    <row r="307" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>1018</v>
       </c>
@@ -16239,8 +16865,10 @@
       <c r="O307" s="7">
         <v>0.12482460987747344</v>
       </c>
-    </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R307" s="1"/>
+      <c r="T307" s="7"/>
+    </row>
+    <row r="308" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>1019</v>
       </c>
@@ -16259,11 +16887,16 @@
       <c r="F308" s="1">
         <v>54</v>
       </c>
+      <c r="G308" s="1">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H308">
-        <v>11.899999999999999</v>
+        <f>17.4-5.5-G308</f>
+        <v>10.799999999999999</v>
       </c>
       <c r="I308" s="7">
-        <v>336.46457319946683</v>
+        <f>PI()*H308*9</f>
+        <v>305.36280592892791</v>
       </c>
       <c r="J308" s="7">
         <v>75.598012937438895</v>
@@ -16283,8 +16916,10 @@
       <c r="O308" s="7">
         <v>-2.9370942606837049</v>
       </c>
-    </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R308" s="1"/>
+      <c r="T308" s="7"/>
+    </row>
+    <row r="309" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>1020</v>
       </c>
@@ -16303,11 +16938,16 @@
       <c r="F309" s="1">
         <v>57</v>
       </c>
+      <c r="G309" s="1">
+        <v>0.9</v>
+      </c>
       <c r="H309">
-        <v>11.899999999999999</v>
+        <f>17.4-5.5-G309</f>
+        <v>10.999999999999998</v>
       </c>
       <c r="I309" s="7">
-        <v>336.46457319946683</v>
+        <f>PI()*H309*9</f>
+        <v>311.01767270538949</v>
       </c>
       <c r="J309" s="7">
         <v>118.67129937853774</v>
@@ -16327,8 +16967,10 @@
       <c r="O309" s="7">
         <v>-3.3113184262650512</v>
       </c>
-    </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R309" s="1"/>
+      <c r="T309" s="7"/>
+    </row>
+    <row r="310" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>1025</v>
       </c>
@@ -16374,8 +17016,10 @@
       <c r="O310" s="7">
         <v>37.794838050011805</v>
       </c>
-    </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R310" s="1"/>
+      <c r="T310" s="7"/>
+    </row>
+    <row r="311" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>1026</v>
       </c>
@@ -16421,8 +17065,10 @@
       <c r="O311" s="7">
         <v>56.451195033025158</v>
       </c>
-    </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R311" s="1"/>
+      <c r="T311" s="7"/>
+    </row>
+    <row r="312" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>1027</v>
       </c>
@@ -16471,8 +17117,10 @@
       <c r="P312">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R312" s="1"/>
+      <c r="T312" s="7"/>
+    </row>
+    <row r="313" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>1028</v>
       </c>
@@ -16521,8 +17169,10 @@
       <c r="P313">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R313" s="1"/>
+      <c r="T313" s="7"/>
+    </row>
+    <row r="314" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>1029</v>
       </c>
@@ -16571,8 +17221,10 @@
       <c r="P314">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R314" s="1"/>
+      <c r="T314" s="7"/>
+    </row>
+    <row r="315" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>1030</v>
       </c>
@@ -16621,8 +17273,10 @@
       <c r="P315">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R315" s="1"/>
+      <c r="T315" s="7"/>
+    </row>
+    <row r="316" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>1031</v>
       </c>
@@ -16671,8 +17325,10 @@
       <c r="P316">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R316" s="1"/>
+      <c r="T316" s="7"/>
+    </row>
+    <row r="317" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>1032</v>
       </c>
@@ -16722,7 +17378,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>1033</v>
       </c>
@@ -16772,7 +17428,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>1034</v>
       </c>
@@ -16821,8 +17477,9 @@
       <c r="P319">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T319" s="7"/>
+    </row>
+    <row r="320" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>1035</v>
       </c>
@@ -16871,8 +17528,9 @@
       <c r="P320">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T320" s="7"/>
+    </row>
+    <row r="321" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>1036</v>
       </c>
@@ -16921,8 +17579,9 @@
       <c r="P321">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T321" s="7"/>
+    </row>
+    <row r="322" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>1037</v>
       </c>
@@ -16971,8 +17630,9 @@
       <c r="P322">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T322" s="7"/>
+    </row>
+    <row r="323" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>1038</v>
       </c>
@@ -17021,8 +17681,10 @@
       <c r="P323">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R323" s="1"/>
+      <c r="T323" s="7"/>
+    </row>
+    <row r="324" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>1039</v>
       </c>
@@ -17071,8 +17733,10 @@
       <c r="P324">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R324" s="1"/>
+      <c r="T324" s="7"/>
+    </row>
+    <row r="325" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>1040</v>
       </c>
@@ -17121,8 +17785,10 @@
       <c r="P325">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R325" s="1"/>
+      <c r="T325" s="7"/>
+    </row>
+    <row r="326" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>1041</v>
       </c>
@@ -17168,8 +17834,10 @@
       <c r="O326" s="7">
         <v>136.42731649587665</v>
       </c>
-    </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R326" s="1"/>
+      <c r="T326" s="7"/>
+    </row>
+    <row r="327" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>1042</v>
       </c>
@@ -17215,8 +17883,10 @@
       <c r="O327" s="7">
         <v>134.13594637595557</v>
       </c>
-    </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R327" s="1"/>
+      <c r="T327" s="7"/>
+    </row>
+    <row r="328" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>1043</v>
       </c>
@@ -17262,8 +17932,10 @@
       <c r="O328" s="7">
         <v>106.86637326560755</v>
       </c>
-    </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R328" s="1"/>
+      <c r="T328" s="7"/>
+    </row>
+    <row r="329" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>1044</v>
       </c>
@@ -17309,8 +17981,10 @@
       <c r="O329" s="7">
         <v>111.13149784526266</v>
       </c>
-    </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R329" s="1"/>
+      <c r="T329" s="7"/>
+    </row>
+    <row r="330" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>1045</v>
       </c>
@@ -17356,8 +18030,10 @@
       <c r="O330" s="7">
         <v>140.59866347118393</v>
       </c>
-    </row>
-    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R330" s="1"/>
+      <c r="T330" s="7"/>
+    </row>
+    <row r="331" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>1046</v>
       </c>
@@ -17403,8 +18079,10 @@
       <c r="O331" s="7">
         <v>161.72153859510883</v>
       </c>
-    </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R331" s="1"/>
+      <c r="T331" s="7"/>
+    </row>
+    <row r="332" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>1051</v>
       </c>
@@ -17450,8 +18128,10 @@
       <c r="O332" s="7" t="e">
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R332" s="1"/>
+      <c r="T332" s="7"/>
+    </row>
+    <row r="333" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>1052</v>
       </c>
@@ -17497,8 +18177,10 @@
       <c r="O333" s="7">
         <v>40.610891934240236</v>
       </c>
-    </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R333" s="1"/>
+      <c r="T333" s="7"/>
+    </row>
+    <row r="334" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>1053</v>
       </c>
@@ -17547,8 +18229,10 @@
       <c r="P334">
         <v>5.33</v>
       </c>
-    </row>
-    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R334" s="1"/>
+      <c r="T334" s="7"/>
+    </row>
+    <row r="335" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>1054</v>
       </c>
@@ -17597,8 +18281,10 @@
       <c r="P335">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R335" s="1"/>
+      <c r="T335" s="7"/>
+    </row>
+    <row r="336" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>1055</v>
       </c>
@@ -17647,8 +18333,10 @@
       <c r="P336">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R336" s="1"/>
+      <c r="T336" s="7"/>
+    </row>
+    <row r="337" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>1056</v>
       </c>
@@ -17697,8 +18385,10 @@
       <c r="P337">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R337" s="1"/>
+      <c r="T337" s="7"/>
+    </row>
+    <row r="338" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>1057</v>
       </c>
@@ -17747,8 +18437,10 @@
       <c r="P338">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R338" s="1"/>
+      <c r="T338" s="7"/>
+    </row>
+    <row r="339" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>1058</v>
       </c>
@@ -17797,8 +18489,10 @@
       <c r="P339">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R339" s="1"/>
+      <c r="T339" s="7"/>
+    </row>
+    <row r="340" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>1059</v>
       </c>
@@ -17847,8 +18541,10 @@
       <c r="P340">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R340" s="1"/>
+      <c r="T340" s="7"/>
+    </row>
+    <row r="341" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>1060</v>
       </c>
@@ -17897,8 +18593,10 @@
       <c r="P341">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R341" s="1"/>
+      <c r="T341" s="7"/>
+    </row>
+    <row r="342" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>1061</v>
       </c>
@@ -17947,8 +18645,10 @@
       <c r="P342">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R342" s="1"/>
+      <c r="T342" s="7"/>
+    </row>
+    <row r="343" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>1062</v>
       </c>
@@ -17998,7 +18698,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>1063</v>
       </c>
@@ -18048,7 +18748,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>1064</v>
       </c>
@@ -18098,7 +18798,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>1065</v>
       </c>
@@ -18148,7 +18848,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>1066</v>
       </c>
@@ -18198,7 +18898,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>1067</v>
       </c>
@@ -18245,7 +18945,7 @@
         <v>122.63372211060911</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>1068</v>
       </c>
@@ -18292,7 +18992,7 @@
         <v>105.66397112347074</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>1069</v>
       </c>
@@ -18339,7 +19039,7 @@
         <v>110.01984303460786</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>1070</v>
       </c>
@@ -18386,7 +19086,7 @@
         <v>122.79252994070264</v>
       </c>
     </row>
-    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>1071</v>
       </c>

</xml_diff>

<commit_message>
Made some statistical calculations, started with the writing the results.
</commit_message>
<xml_diff>
--- a/index/data/incubationgraph.xlsx
+++ b/index/data/incubationgraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AD8FE3-C391-4D44-8D5C-1CEA2B6B11FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA3DCC8-7949-44AB-8A39-EFCB2030ACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8251E3DC-A7BA-4CC3-B3AA-E4750F949FDE}"/>
   </bookViews>
@@ -1100,15 +1100,6 @@
     <t>BL-D3.2-inc-21</t>
   </si>
   <si>
-    <t>FeII(uM)</t>
-  </si>
-  <si>
-    <t>FeTot(uM)</t>
-  </si>
-  <si>
-    <t>FeIII(uM)</t>
-  </si>
-  <si>
     <t>NH4</t>
   </si>
   <si>
@@ -1184,9 +1175,6 @@
     <t>volume_(ml)</t>
   </si>
   <si>
-    <t>Preal(uM)</t>
-  </si>
-  <si>
     <t>DO(mg/L)</t>
   </si>
   <si>
@@ -1194,6 +1182,18 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>FeTot</t>
+  </si>
+  <si>
+    <t>FeIII</t>
+  </si>
+  <si>
+    <t>Preal</t>
+  </si>
+  <si>
+    <t>FeII</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:T353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V328" sqref="V328"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,49 +1677,49 @@
         <v>144</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>357</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1777,7 +1777,7 @@
         <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -2847,7 +2847,7 @@
         <v>159</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -3904,7 +3904,7 @@
         <v>172</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -5007,7 +5007,7 @@
         <v>185</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D69" s="1">
         <v>2</v>
@@ -6124,7 +6124,7 @@
         <v>198</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -7200,7 +7200,7 @@
         <v>211</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D113" s="1">
         <v>0</v>
@@ -8280,7 +8280,7 @@
         <v>224</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D135" s="1">
         <v>0</v>
@@ -9340,7 +9340,7 @@
         <v>843</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>63</v>
@@ -9372,10 +9372,10 @@
         <v>844</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D157" s="1">
         <v>2</v>
@@ -9421,7 +9421,7 @@
         <v>845</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>66</v>
@@ -9470,7 +9470,7 @@
         <v>846</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>68</v>
@@ -9522,7 +9522,7 @@
         <v>847</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>70</v>
@@ -9574,7 +9574,7 @@
         <v>848</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>64</v>
@@ -9626,7 +9626,7 @@
         <v>849</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>65</v>
@@ -9678,7 +9678,7 @@
         <v>850</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>67</v>
@@ -9730,7 +9730,7 @@
         <v>851</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>69</v>
@@ -9782,7 +9782,7 @@
         <v>852</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>71</v>
@@ -9834,7 +9834,7 @@
         <v>853</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>238</v>
@@ -9886,7 +9886,7 @@
         <v>854</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>239</v>
@@ -9938,7 +9938,7 @@
         <v>855</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>240</v>
@@ -9990,7 +9990,7 @@
         <v>856</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>241</v>
@@ -10042,7 +10042,7 @@
         <v>857</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>242</v>
@@ -10094,7 +10094,7 @@
         <v>858</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>243</v>
@@ -10146,7 +10146,7 @@
         <v>859</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>244</v>
@@ -10195,7 +10195,7 @@
         <v>860</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>245</v>
@@ -10244,7 +10244,7 @@
         <v>861</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>246</v>
@@ -10293,7 +10293,7 @@
         <v>862</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>247</v>
@@ -10342,7 +10342,7 @@
         <v>863</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>248</v>
@@ -10391,7 +10391,7 @@
         <v>864</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>249</v>
@@ -10492,7 +10492,7 @@
         <v>250</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D179" s="1">
         <v>0</v>
@@ -11574,7 +11574,7 @@
         <v>263</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D201" s="1">
         <v>0</v>
@@ -12648,7 +12648,7 @@
         <v>276</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D223" s="1">
         <v>0</v>
@@ -13743,7 +13743,7 @@
         <v>289</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D245" s="1">
         <v>1</v>
@@ -14863,7 +14863,7 @@
         <v>302</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D267" s="1">
         <v>0</v>
@@ -15945,7 +15945,7 @@
         <v>315</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D289" s="1">
         <v>0</v>
@@ -17027,7 +17027,7 @@
         <v>328</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D311" s="1">
         <v>0</v>
@@ -18139,7 +18139,7 @@
         <v>341</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D333" s="1">
         <v>1</v>
@@ -19199,7 +19199,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Calculated benthic fluxes and benthic flux plot.
</commit_message>
<xml_diff>
--- a/index/data/incubationgraph.xlsx
+++ b/index/data/incubationgraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA3DCC8-7949-44AB-8A39-EFCB2030ACF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263947A9-328A-4D22-AB3A-30870EFEFA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8251E3DC-A7BA-4CC3-B3AA-E4750F949FDE}"/>
   </bookViews>
@@ -1163,21 +1163,9 @@
     <t>cmevap</t>
   </si>
   <si>
-    <t>delay(days)</t>
-  </si>
-  <si>
     <t>samplenr</t>
   </si>
   <si>
-    <t>water_column_(cm)</t>
-  </si>
-  <si>
-    <t>volume_(ml)</t>
-  </si>
-  <si>
-    <t>DO(mg/L)</t>
-  </si>
-  <si>
     <t>H2SuM</t>
   </si>
   <si>
@@ -1194,6 +1182,18 @@
   </si>
   <si>
     <t>FeII</t>
+  </si>
+  <si>
+    <t>volume_ml</t>
+  </si>
+  <si>
+    <t>water_column_cm</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>DO</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:T353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="V15" sqref="V14:V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1672,7 @@
     <col min="15" max="15" width="9" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>144</v>
       </c>
@@ -1680,46 +1680,46 @@
         <v>356</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>374</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>380</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>384</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>354</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed some bugs, added some figures
</commit_message>
<xml_diff>
--- a/index/data/incubationgraph.xlsx
+++ b/index/data/incubationgraph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF33398-70FA-4752-BC84-1B969BCEEB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176CFAF-62A9-44D0-9DCC-E2DC030DE531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8251E3DC-A7BA-4CC3-B3AA-E4750F949FDE}"/>
   </bookViews>
@@ -1121,9 +1121,6 @@
     <t>BL-A3.1-inc-1</t>
   </si>
   <si>
-    <t>BL-A3.2-in-1</t>
-  </si>
-  <si>
     <t>BL-B2.1-inc-1</t>
   </si>
   <si>
@@ -1194,6 +1191,9 @@
   </si>
   <si>
     <t>DO</t>
+  </si>
+  <si>
+    <t>BL-A3.2-inc-1</t>
   </si>
 </sst>
 </file>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3502AA23-6217-443D-8F96-C11B8D580A31}">
   <dimension ref="A1:T353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="V15" sqref="V14:V15"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,46 +1680,46 @@
         <v>356</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="11" t="s">
         <v>379</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>380</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>354</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -5007,7 +5007,7 @@
         <v>185</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="D69" s="1">
         <v>2</v>
@@ -6124,7 +6124,7 @@
         <v>198</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -7200,7 +7200,7 @@
         <v>211</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D113" s="1">
         <v>0</v>
@@ -8280,7 +8280,7 @@
         <v>224</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D135" s="1">
         <v>0</v>
@@ -9375,7 +9375,7 @@
         <v>357</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D157" s="1">
         <v>2</v>
@@ -10492,7 +10492,7 @@
         <v>250</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D179" s="1">
         <v>0</v>
@@ -11574,7 +11574,7 @@
         <v>263</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D201" s="1">
         <v>0</v>
@@ -12648,7 +12648,7 @@
         <v>276</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D223" s="1">
         <v>0</v>
@@ -13743,7 +13743,7 @@
         <v>289</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D245" s="1">
         <v>1</v>
@@ -14863,7 +14863,7 @@
         <v>302</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D267" s="1">
         <v>0</v>
@@ -15945,7 +15945,7 @@
         <v>315</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D289" s="1">
         <v>0</v>
@@ -17027,7 +17027,7 @@
         <v>328</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D311" s="1">
         <v>0</v>
@@ -18139,7 +18139,7 @@
         <v>341</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D333" s="1">
         <v>1</v>

</xml_diff>